<commit_message>
auto commit via batch
</commit_message>
<xml_diff>
--- a/Docs/Results.xlsx
+++ b/Docs/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughm\OneDrive\UQ\PHYS4070\Assignments\Assignment1\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0CD311-97BD-46A3-A0F7-1BB4AB4BC05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F78CC38-3CB8-4870-8DAE-3B9F54B438B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15705" activeTab="4" xr2:uid="{B201E39B-ED22-462E-BB3A-90A37975CEA0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{B201E39B-ED22-462E-BB3A-90A37975CEA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Q1Short" sheetId="6" r:id="rId3"/>
     <sheet name="Q2" sheetId="5" r:id="rId4"/>
     <sheet name="Q3" sheetId="4" r:id="rId5"/>
-    <sheet name="Q4" sheetId="3" r:id="rId6"/>
+    <sheet name="Alts" sheetId="7" r:id="rId6"/>
+    <sheet name="Q4" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>T</t>
   </si>
@@ -130,6 +131,21 @@
   <si>
     <t>e2p</t>
   </si>
+  <si>
+    <t>182983       0.02</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>e_2p</t>
+  </si>
+  <si>
+    <t>om</t>
+  </si>
 </sst>
 </file>
 
@@ -140,8 +156,8 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.0E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -205,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,11 +236,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -3821,14 +3836,14 @@
       <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="3" max="3" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -3839,7 +3854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -3850,7 +3865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3861,7 +3876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -3873,7 +3888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -3885,7 +3900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -3911,9 +3926,9 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3927,7 +3942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3941,7 +3956,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3961,7 +3976,7 @@
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3978,7 +3993,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3995,7 +4010,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4012,7 +4027,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4029,7 +4044,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4046,7 +4061,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4063,7 +4078,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4080,7 +4095,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4097,7 +4112,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -4114,7 +4129,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -4127,7 +4142,7 @@
       </c>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -4146,7 +4161,7 @@
         <v>1.67441</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -4165,7 +4180,7 @@
         <v>4.1689999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -4184,7 +4199,7 @@
         <v>7.6682399999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -4203,7 +4218,7 @@
         <v>12.168799999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -4222,7 +4237,7 @@
         <v>17.669799999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7</v>
       </c>
@@ -4241,7 +4256,7 @@
         <v>24.1707</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>8</v>
       </c>
@@ -4260,7 +4275,7 @@
         <v>31.671500000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9</v>
       </c>
@@ -4279,7 +4294,7 @@
         <v>40.172400000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10</v>
       </c>
@@ -4298,7 +4313,7 @@
         <v>49.673200000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E24" s="9"/>
     </row>
   </sheetData>
@@ -4316,36 +4331,36 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="15">
         <v>-4.5302899999999999</v>
       </c>
       <c r="C2" s="11"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="11">
         <v>-1.1287799999999999</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <v>-1.125</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4358,7 +4373,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4371,7 +4386,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4384,7 +4399,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4397,7 +4412,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4410,7 +4425,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4423,7 +4438,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4436,7 +4451,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4449,73 +4464,73 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E24" s="9"/>
     </row>
   </sheetData>
@@ -4532,13 +4547,13 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -4555,7 +4570,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4575,7 +4590,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4592,7 +4607,7 @@
         <v>-0.13006699999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4609,7 +4624,7 @@
         <v>-5.7222500000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4635,7 +4650,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4666,7 +4681,7 @@
         <v>6.7909999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4697,11 +4712,11 @@
         <f>2/3*$H$10^2*J6^3*10.71</f>
         <v>5.5363943224085263E-2</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4736,7 +4751,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4753,7 +4768,7 @@
         <v>-7.1633E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4776,7 +4791,7 @@
         <v>4.9758101963229304</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4802,13 +4817,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F76B73-EEE8-4A17-85F0-7AB4FA154F64}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -4822,7 +4837,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4832,11 +4847,11 @@
       <c r="C2" s="11">
         <v>-0.198411</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="17">
         <v>0.55557999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4846,11 +4861,11 @@
       <c r="C3" s="11">
         <v>-0.178288</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>0.47621400000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4860,11 +4875,11 @@
       <c r="C4" s="11">
         <v>-0.18506</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>0.13208300000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4874,11 +4889,11 @@
       <c r="C5" s="11">
         <v>-0.182251</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>5.9874200000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4888,11 +4903,11 @@
       <c r="C6" s="11">
         <v>-0.18334300000000001</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>2.25075E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4902,11 +4917,11 @@
       <c r="C7" s="11">
         <v>-0.18290600000000001</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>9.1239600000000004E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4916,11 +4931,11 @@
       <c r="C8" s="11">
         <v>-0.18307899999999999</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>3.5902199999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4930,11 +4945,11 @@
       <c r="C9" s="11">
         <v>-0.18301000000000001</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>1.4295499999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4944,11 +4959,11 @@
       <c r="C10" s="11">
         <v>-0.18303800000000001</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>5.6654999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4958,11 +4973,11 @@
       <c r="C11" s="11">
         <v>-0.183027</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>2.2494999999999999E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4972,11 +4987,11 @@
       <c r="C12" s="11">
         <v>-0.183031</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>8.9251200000000004E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4986,11 +5001,11 @@
       <c r="C13" s="11">
         <v>-0.183029</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>3.54217E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5000,11 +5015,11 @@
       <c r="C14" s="11">
         <v>-0.18303</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>1.40564E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5014,11 +5029,11 @@
       <c r="C15" s="11">
         <v>-0.18303</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>5.5782600000000002E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5028,11 +5043,11 @@
       <c r="C16" s="11">
         <v>-0.18303</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="17">
         <v>2.21368E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5042,11 +5057,11 @@
       <c r="C17" s="11">
         <v>-0.18303</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>8.7848599999999997E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -5056,7 +5071,7 @@
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -5079,7 +5094,7 @@
         <v>1.5327917498931085</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -5102,7 +5117,7 @@
         <v>0.88435172607247192</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
@@ -5125,7 +5140,7 @@
         <v>0.61859635884802899</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -5148,7 +5163,7 @@
         <v>0.47427707321274476</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -5171,7 +5186,7 @@
         <v>0.38413359007805858</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>7</v>
       </c>
@@ -5194,7 +5209,7 @@
         <v>0.32405570300663722</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8</v>
       </c>
@@ -5217,7 +5232,7 @@
         <v>0.32873077490049629</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>9</v>
       </c>
@@ -5240,7 +5255,7 @@
         <v>0.58598156197403239</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
@@ -5263,7 +5278,7 @@
         <v>2.2146976916386492</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -5277,19 +5292,602 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A81FF6-EBE2-4C4C-B878-872EFF19CAD7}">
+  <dimension ref="A2:N29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1.8357699999999999</v>
+      </c>
+      <c r="C2">
+        <v>-0.19784199999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.55236300000000005</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>-1.8357699999999999</v>
+      </c>
+      <c r="M2">
+        <v>-0.19784199999999999</v>
+      </c>
+      <c r="N2">
+        <v>0.55236300000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-1.2480199999999999</v>
+      </c>
+      <c r="C3">
+        <v>-0.177956</v>
+      </c>
+      <c r="D3">
+        <v>0.47094799999999998</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>-1.2480199999999999</v>
+      </c>
+      <c r="M3">
+        <v>-0.177956</v>
+      </c>
+      <c r="N3">
+        <v>0.47094799999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1.4372400000000001</v>
+      </c>
+      <c r="C4">
+        <v>-0.184692</v>
+      </c>
+      <c r="D4">
+        <v>0.131656</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>-1.4372400000000001</v>
+      </c>
+      <c r="M4">
+        <v>-0.184692</v>
+      </c>
+      <c r="N4">
+        <v>0.131656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-1.35602</v>
+      </c>
+      <c r="C5">
+        <v>-0.18188699999999999</v>
+      </c>
+      <c r="D5">
+        <v>5.9900399999999999E-2</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>-1.35602</v>
+      </c>
+      <c r="M5">
+        <v>-0.18188699999999999</v>
+      </c>
+      <c r="N5">
+        <v>5.9900399999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1.3874</v>
+      </c>
+      <c r="C6">
+        <v>-0.18298300000000001</v>
+      </c>
+      <c r="D6">
+        <v>2.26197E-2</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f>-1.3874 -0</f>
+        <v>-1.3874</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6">
+        <v>26197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-1.37473</v>
+      </c>
+      <c r="C7">
+        <v>-0.18254300000000001</v>
+      </c>
+      <c r="D7">
+        <v>9.2110500000000001E-3</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>-1.37473</v>
+      </c>
+      <c r="M7">
+        <v>-0.18254300000000001</v>
+      </c>
+      <c r="N7">
+        <v>9.2110500000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-1.3797600000000001</v>
+      </c>
+      <c r="C8">
+        <v>-0.18271799999999999</v>
+      </c>
+      <c r="D8">
+        <v>3.6404699999999998E-3</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>-1.3797600000000001</v>
+      </c>
+      <c r="M8">
+        <v>-0.18271799999999999</v>
+      </c>
+      <c r="N8">
+        <v>3.6404699999999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-1.37775</v>
+      </c>
+      <c r="C9">
+        <v>-0.182648</v>
+      </c>
+      <c r="D9">
+        <v>1.4561000000000001E-3</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>-1.37775</v>
+      </c>
+      <c r="M9">
+        <v>-0.182648</v>
+      </c>
+      <c r="N9">
+        <v>1.4561000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-1.3785499999999999</v>
+      </c>
+      <c r="C10">
+        <v>-0.18267600000000001</v>
+      </c>
+      <c r="D10">
+        <v>5.79642E-4</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="L10">
+        <v>-1.3785499999999999</v>
+      </c>
+      <c r="M10">
+        <v>-0.18267600000000001</v>
+      </c>
+      <c r="N10">
+        <v>5.79642E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-1.3782300000000001</v>
+      </c>
+      <c r="C11">
+        <v>-0.18266499999999999</v>
+      </c>
+      <c r="D11">
+        <v>2.3118100000000001E-4</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>-1.3782300000000001</v>
+      </c>
+      <c r="M11">
+        <v>-0.18266499999999999</v>
+      </c>
+      <c r="N11">
+        <v>2.3118100000000001E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-1.37836</v>
+      </c>
+      <c r="C12">
+        <v>-0.182669</v>
+      </c>
+      <c r="D12" s="6">
+        <v>9.2133399999999994E-5</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>-1.37836</v>
+      </c>
+      <c r="M12">
+        <v>-0.182669</v>
+      </c>
+      <c r="N12" s="6">
+        <v>9.2133399999999994E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-1.3783099999999999</v>
+      </c>
+      <c r="C13">
+        <v>-0.182667</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3.6729200000000001E-5</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>-1.3783099999999999</v>
+      </c>
+      <c r="M13">
+        <v>-0.182667</v>
+      </c>
+      <c r="N13" s="6">
+        <v>3.6729200000000001E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-1.3783300000000001</v>
+      </c>
+      <c r="C14">
+        <v>-0.182668</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1.46405E-5</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>-1.3783300000000001</v>
+      </c>
+      <c r="M14">
+        <v>-0.182668</v>
+      </c>
+      <c r="N14" s="6">
+        <v>1.46405E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <v>-1.37832</v>
+      </c>
+      <c r="C15" s="7">
+        <v>-0.182668</v>
+      </c>
+      <c r="D15" s="8">
+        <v>5.8360499999999998E-6</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+      <c r="L15">
+        <v>-1.37832</v>
+      </c>
+      <c r="M15">
+        <v>-0.182668</v>
+      </c>
+      <c r="N15" s="6">
+        <v>5.8360499999999998E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>-2.8016399999999999</v>
+      </c>
+      <c r="C16">
+        <v>-0.19969899999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.50802999999999998</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+      <c r="L16">
+        <v>-1.37832</v>
+      </c>
+      <c r="M16">
+        <v>-0.182668</v>
+      </c>
+      <c r="N16" s="6">
+        <v>2.3263500000000002E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" ref="A17:A23" si="0">A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>-2.72567</v>
+      </c>
+      <c r="C17">
+        <v>-0.19613900000000001</v>
+      </c>
+      <c r="D17">
+        <v>2.7873100000000001E-2</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="L17">
+        <v>-1.37832</v>
+      </c>
+      <c r="M17">
+        <v>-0.182668</v>
+      </c>
+      <c r="N17" s="6">
+        <v>9.27327E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>-2.71698</v>
+      </c>
+      <c r="C18">
+        <v>-0.19594800000000001</v>
+      </c>
+      <c r="D18">
+        <v>3.1977500000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>-2.71583</v>
+      </c>
+      <c r="C19">
+        <v>-0.19592499999999999</v>
+      </c>
+      <c r="D19">
+        <v>4.2237200000000001E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>-2.7156699999999998</v>
+      </c>
+      <c r="C20">
+        <v>-0.19592200000000001</v>
+      </c>
+      <c r="D20" s="6">
+        <v>5.7841799999999999E-5</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>-2.7156500000000001</v>
+      </c>
+      <c r="C21">
+        <v>-0.19592200000000001</v>
+      </c>
+      <c r="D21" s="6">
+        <v>8.0487999999999999E-6</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>-2.7156500000000001</v>
+      </c>
+      <c r="C22">
+        <v>-0.19592200000000001</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1.1318600000000001E-6</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>-2.7156500000000001</v>
+      </c>
+      <c r="C23">
+        <v>-0.19592200000000001</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1.6042999999999999E-7</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="11">
+        <v>-0.182668</v>
+      </c>
+      <c r="C26" s="11">
+        <v>-0.19592200000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="11">
+        <v>-0.12748599999999999</v>
+      </c>
+      <c r="C27" s="11">
+        <v>-0.129078</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="11">
+        <f>ABS(B26-B27)</f>
+        <v>5.5182000000000009E-2</v>
+      </c>
+      <c r="C28" s="11">
+        <f>ABS(C26-C27)</f>
+        <v>6.6844000000000015E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="9">
+        <v>43.878</v>
+      </c>
+      <c r="C29" s="9">
+        <v>27.540700000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F970714-F316-49B5-A51D-04C9C8F44B69}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -5303,7 +5901,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5317,7 +5915,7 @@
         <v>0.55557999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5331,7 +5929,7 @@
         <v>0.47621400000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5345,7 +5943,7 @@
         <v>0.13208300000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5359,7 +5957,7 @@
         <v>5.9874200000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5373,7 +5971,7 @@
         <v>2.25075E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5387,7 +5985,7 @@
         <v>9.1239600000000004E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5401,7 +5999,7 @@
         <v>3.5902199999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5415,7 +6013,7 @@
         <v>1.4295499999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5429,7 +6027,7 @@
         <v>5.6654999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5443,7 +6041,7 @@
         <v>2.2494999999999999E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5457,7 +6055,7 @@
         <v>8.9251200000000004E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5471,7 +6069,7 @@
         <v>3.54217E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5485,21 +6083,21 @@
         <v>1.40564E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="18">
         <v>-1.38398</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="18">
         <v>-0.18303</v>
       </c>
       <c r="D15" s="8">
         <v>5.5782600000000002E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>A15+1</f>
         <v>15</v>
@@ -5514,7 +6112,7 @@
         <v>0.50795999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" ref="A17:A23" si="0">A16+1</f>
         <v>16</v>
@@ -5529,7 +6127,7 @@
         <v>2.7718799999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5544,7 +6142,7 @@
         <v>3.19235E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5559,7 +6157,7 @@
         <v>4.2294099999999997E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5574,7 +6172,7 @@
         <v>5.8037200000000001E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5589,7 +6187,7 @@
         <v>8.0862000000000006E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5604,7 +6202,7 @@
         <v>1.1378999999999999E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5619,7 +6217,7 @@
         <v>1.61326E-7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -5629,7 +6227,7 @@
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -5652,7 +6250,7 @@
         <v>1.7313573759724132</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -5675,7 +6273,7 @@
         <v>0.90737410005353591</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -5698,7 +6296,7 @@
         <v>0.6292271370662389</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -5721,7 +6319,7 @@
         <v>0.48040740854184438</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -5744,7 +6342,7 @@
         <v>0.38811490880715854</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>7</v>
       </c>
@@ -5767,7 +6365,7 @@
         <v>0.32651479138479544</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8</v>
       </c>
@@ -5790,7 +6388,7 @@
         <v>0.32439716002273361</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>9</v>
       </c>
@@ -5813,7 +6411,7 @@
         <v>0.56073036960912315</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10</v>
       </c>
@@ -5836,7 +6434,7 @@
         <v>1.9622482738537388</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>18</v>
       </c>

</xml_diff>